<commit_message>
1103 features and random forest
</commit_message>
<xml_diff>
--- a/round2/20151102.xlsx
+++ b/round2/20151102.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19580" yWindow="0" windowWidth="20840" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="21600" yWindow="0" windowWidth="17340" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>yreal</t>
   </si>
@@ -52,16 +52,56 @@
   </si>
   <si>
     <t>55/25/3/2.5</t>
+  </si>
+  <si>
+    <t>55/30/3/2</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>RF2</t>
+  </si>
+  <si>
+    <t>RF1</t>
+  </si>
+  <si>
+    <t>sql</t>
+  </si>
+  <si>
+    <t>RF3</t>
+  </si>
+  <si>
+    <t>100-N</t>
+  </si>
+  <si>
+    <t>RF4</t>
+  </si>
+  <si>
+    <t>800-N</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>LR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,68 +146,117 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -195,6 +284,30 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -222,6 +335,30 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -551,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -959,7 +1096,7 @@
         <v>372023</v>
       </c>
       <c r="H35">
-        <f>C35+10*D35+50*E35+100*F35+200*G35</f>
+        <f t="shared" ref="H35:H43" si="1">C35+10*D35+50*E35+100*F35+200*G35</f>
         <v>300967448</v>
       </c>
     </row>
@@ -980,7 +1117,7 @@
         <v>333054</v>
       </c>
       <c r="H36">
-        <f>C36+10*D36+50*E36+100*F36+200*G36</f>
+        <f t="shared" si="1"/>
         <v>213401572</v>
       </c>
       <c r="I36">
@@ -1005,7 +1142,7 @@
         <v>333054</v>
       </c>
       <c r="H37">
-        <f>C37+10*D37+50*E37+100*F37+200*G37</f>
+        <f t="shared" si="1"/>
         <v>224267580</v>
       </c>
       <c r="I37">
@@ -1033,7 +1170,7 @@
         <v>323316</v>
       </c>
       <c r="H38">
-        <f>C38+10*D38+50*E38+100*F38+200*G38</f>
+        <f t="shared" si="1"/>
         <v>224279780</v>
       </c>
       <c r="I38">
@@ -1061,7 +1198,7 @@
         <v>321177</v>
       </c>
       <c r="H39">
-        <f>C39+10*D39+50*E39+100*F39+200*G39</f>
+        <f t="shared" si="1"/>
         <v>224227280</v>
       </c>
     </row>
@@ -1086,7 +1223,7 @@
         <v>327360</v>
       </c>
       <c r="H40" s="1">
-        <f>C40+10*D40+50*E40+100*F40+200*G40</f>
+        <f t="shared" si="1"/>
         <v>224301680</v>
       </c>
       <c r="I40" s="1">
@@ -1114,13 +1251,278 @@
         <v>323316</v>
       </c>
       <c r="H41">
-        <f>C41+10*D41+50*E41+100*F41+200*G41</f>
+        <f t="shared" si="1"/>
         <v>223587630</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>10</v>
+      </c>
+      <c r="C42">
+        <v>103663134</v>
+      </c>
+      <c r="D42">
+        <v>103862</v>
+      </c>
+      <c r="E42" s="1">
+        <v>876998</v>
+      </c>
+      <c r="F42" s="1">
+        <v>103161</v>
+      </c>
+      <c r="G42" s="1">
+        <v>327360</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="1"/>
+        <v>224339754</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="1">
+        <v>102516230</v>
+      </c>
+      <c r="D43" s="1">
+        <v>214745</v>
+      </c>
+      <c r="E43">
+        <v>974816</v>
+      </c>
+      <c r="F43">
+        <v>88017</v>
+      </c>
+      <c r="G43" s="1">
+        <v>327360</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="1"/>
+        <v>227678180</v>
+      </c>
+      <c r="I43" s="1">
+        <f>H43/$H$35</f>
+        <v>0.7564877248784726</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="E46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" t="s">
+        <v>20</v>
+      </c>
+      <c r="H47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48">
+        <v>21385661</v>
+      </c>
+      <c r="B48">
+        <v>20502785</v>
+      </c>
+      <c r="C48">
+        <v>20724442</v>
+      </c>
+      <c r="D48">
+        <v>21340331</v>
+      </c>
+      <c r="E48">
+        <v>20618296</v>
+      </c>
+      <c r="F48">
+        <v>20619651</v>
+      </c>
+      <c r="G48">
+        <v>7837394</v>
+      </c>
+      <c r="H48">
+        <v>20710004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>289322</v>
+      </c>
+      <c r="B49">
+        <v>42782</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>16</v>
+      </c>
+      <c r="E49">
+        <v>15</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>257785</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>299938</v>
+      </c>
+      <c r="B50">
+        <v>195288</v>
+      </c>
+      <c r="C50">
+        <v>249681</v>
+      </c>
+      <c r="D50">
+        <v>133074</v>
+      </c>
+      <c r="E50">
+        <v>253541</v>
+      </c>
+      <c r="F50">
+        <v>253062</v>
+      </c>
+      <c r="G50">
+        <v>100536</v>
+      </c>
+      <c r="H50">
+        <v>205930</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51">
+        <v>60493</v>
+      </c>
+      <c r="B51">
+        <v>17726</v>
+      </c>
+      <c r="C51">
+        <v>83</v>
+      </c>
+      <c r="D51">
+        <v>647</v>
+      </c>
+      <c r="E51">
+        <v>1528</v>
+      </c>
+      <c r="F51">
+        <v>17</v>
+      </c>
+      <c r="G51">
+        <v>7609</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52">
+        <v>74789</v>
+      </c>
+      <c r="B52">
+        <v>65890</v>
+      </c>
+      <c r="C52">
+        <v>62220</v>
+      </c>
+      <c r="D52">
+        <v>43875</v>
+      </c>
+      <c r="E52">
+        <v>65820</v>
+      </c>
+      <c r="F52">
+        <v>66566</v>
+      </c>
+      <c r="G52">
+        <v>30482</v>
+      </c>
+      <c r="H52">
+        <v>64796</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53">
+        <f>A48+A49*10+A50*50+A51*100+A52*200</f>
+        <v>60282881</v>
+      </c>
+      <c r="B53">
+        <f>B48+B49*10+B50*50+B51*100+B52*200</f>
+        <v>45645605</v>
+      </c>
+      <c r="C53">
+        <f>C48+C49*10+C50*50+C51*100+C52*200</f>
+        <v>45660802</v>
+      </c>
+      <c r="D53">
+        <f>D48+D49*10+D50*50+D51*100+D52*200</f>
+        <v>36833891</v>
+      </c>
+      <c r="E53">
+        <f>E48+E49*10+E50*50+E51*100+E52*200</f>
+        <v>46612296</v>
+      </c>
+      <c r="F53">
+        <f>F48+F49*10+F50*50+F51*100+F52*200</f>
+        <v>46587661</v>
+      </c>
+      <c r="G53">
+        <f>G48+G49*10+G50*50+G51*100+G52*200</f>
+        <v>22299344</v>
+      </c>
+      <c r="H53">
+        <f>H48+H49*10+H50*50+H51*100+H52*200</f>
+        <v>43965704</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="B54">
+        <f>B53/$A$53</f>
+        <v>0.75719017145182566</v>
+      </c>
+      <c r="C54">
+        <f>C53/$A$53</f>
+        <v>0.75744226623807176</v>
+      </c>
+      <c r="E54">
+        <f>E53/$A$53</f>
+        <v>0.77322608386948199</v>
+      </c>
+      <c r="F54">
+        <f>F53/$A$53</f>
+        <v>0.77281742722282964</v>
+      </c>
+      <c r="G54">
+        <f>G53/$A$53</f>
+        <v>0.36991171672767265</v>
+      </c>
+      <c r="H54">
+        <f>H53/$A$53</f>
+        <v>0.72932320537235107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final commit for competition
</commit_message>
<xml_diff>
--- a/round2/20151102.xlsx
+++ b/round2/20151102.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>yreal</t>
   </si>
@@ -85,6 +85,30 @@
   </si>
   <si>
     <t>LR</t>
+  </si>
+  <si>
+    <t>RF5</t>
+  </si>
+  <si>
+    <t>100-20</t>
+  </si>
+  <si>
+    <t>100-30</t>
+  </si>
+  <si>
+    <t>ypred</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>combine1</t>
+  </si>
+  <si>
+    <t>combine2</t>
+  </si>
+  <si>
+    <t>combine3</t>
   </si>
 </sst>
 </file>
@@ -146,8 +170,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -256,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="123">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -308,6 +352,16 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -359,6 +413,16 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -688,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="G37" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1079,7 +1143,7 @@
         <v>99154897</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:15">
       <c r="C35">
         <v>106921008</v>
       </c>
@@ -1100,7 +1164,7 @@
         <v>300967448</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:15">
       <c r="C36">
         <v>97429982</v>
       </c>
@@ -1125,7 +1189,7 @@
         <v>0.70905200352431474</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:15">
       <c r="C37">
         <v>102516230</v>
       </c>
@@ -1150,7 +1214,7 @@
         <v>0.74515560234274902</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1178,7 +1242,7 @@
         <v>0.74519613828801845</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1202,7 +1266,7 @@
         <v>224227280</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:15">
       <c r="A40" s="1" t="s">
         <v>8</v>
       </c>
@@ -1231,7 +1295,7 @@
         <v>0.74526890363239551</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1255,7 +1319,7 @@
         <v>223587630</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1279,7 +1343,7 @@
         <v>224339754</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:15">
       <c r="A43" s="2" t="s">
         <v>11</v>
       </c>
@@ -1307,15 +1371,33 @@
         <v>0.7564877248784726</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:15">
       <c r="E46" t="s">
         <v>17</v>
       </c>
       <c r="F46" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
+      <c r="I46" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K46" t="s">
+        <v>24</v>
+      </c>
+      <c r="M46" t="s">
+        <v>27</v>
+      </c>
+      <c r="N46" t="s">
+        <v>28</v>
+      </c>
+      <c r="O46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -1340,8 +1422,11 @@
       <c r="H47" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="I47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48">
         <v>21385661</v>
       </c>
@@ -1366,8 +1451,26 @@
       <c r="H48">
         <v>20710004</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48">
+        <v>20627948</v>
+      </c>
+      <c r="J48">
+        <v>20646694</v>
+      </c>
+      <c r="K48">
+        <v>20639809</v>
+      </c>
+      <c r="L48">
+        <v>20650981</v>
+      </c>
+      <c r="M48">
+        <v>20502787</v>
+      </c>
+      <c r="N48">
+        <v>20502781</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49">
         <v>289322</v>
       </c>
@@ -1389,8 +1492,26 @@
       <c r="G49">
         <v>257785</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49">
+        <v>7</v>
+      </c>
+      <c r="J49">
+        <v>1119</v>
+      </c>
+      <c r="K49">
+        <v>439</v>
+      </c>
+      <c r="L49">
+        <v>23</v>
+      </c>
+      <c r="M49">
+        <v>42782</v>
+      </c>
+      <c r="N49">
+        <v>13118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50">
         <v>299938</v>
       </c>
@@ -1415,8 +1536,26 @@
       <c r="H50">
         <v>205930</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50">
+        <v>254352</v>
+      </c>
+      <c r="J50">
+        <v>255138</v>
+      </c>
+      <c r="K50">
+        <v>257051</v>
+      </c>
+      <c r="L50">
+        <v>256164</v>
+      </c>
+      <c r="M50">
+        <v>195288</v>
+      </c>
+      <c r="N50">
+        <v>254329</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51">
         <v>60493</v>
       </c>
@@ -1438,8 +1577,26 @@
       <c r="G51">
         <v>7609</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="I51">
+        <v>2398</v>
+      </c>
+      <c r="J51">
+        <v>1831</v>
+      </c>
+      <c r="K51">
+        <v>1075</v>
+      </c>
+      <c r="L51">
+        <v>746</v>
+      </c>
+      <c r="M51">
+        <v>17576</v>
+      </c>
+      <c r="N51">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52">
         <v>74789</v>
       </c>
@@ -1464,42 +1621,84 @@
       <c r="H52">
         <v>64796</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="I52">
+        <v>65001</v>
+      </c>
+      <c r="J52">
+        <v>65086</v>
+      </c>
+      <c r="K52">
+        <v>64858</v>
+      </c>
+      <c r="L52">
+        <v>65385</v>
+      </c>
+      <c r="M52">
+        <v>66052</v>
+      </c>
+      <c r="N52">
+        <v>66052</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53">
-        <f>A48+A49*10+A50*50+A51*100+A52*200</f>
+        <f t="shared" ref="A53:N53" si="2">A48+A49*10+A50*50+A51*100+A52*200</f>
         <v>60282881</v>
       </c>
       <c r="B53">
-        <f>B48+B49*10+B50*50+B51*100+B52*200</f>
+        <f t="shared" si="2"/>
         <v>45645605</v>
       </c>
       <c r="C53">
-        <f>C48+C49*10+C50*50+C51*100+C52*200</f>
+        <f t="shared" si="2"/>
         <v>45660802</v>
       </c>
       <c r="D53">
-        <f>D48+D49*10+D50*50+D51*100+D52*200</f>
+        <f t="shared" si="2"/>
         <v>36833891</v>
       </c>
       <c r="E53">
-        <f>E48+E49*10+E50*50+E51*100+E52*200</f>
+        <f t="shared" si="2"/>
         <v>46612296</v>
       </c>
       <c r="F53">
-        <f>F48+F49*10+F50*50+F51*100+F52*200</f>
+        <f t="shared" si="2"/>
         <v>46587661</v>
       </c>
       <c r="G53">
-        <f>G48+G49*10+G50*50+G51*100+G52*200</f>
+        <f t="shared" si="2"/>
         <v>22299344</v>
       </c>
       <c r="H53">
-        <f>H48+H49*10+H50*50+H51*100+H52*200</f>
+        <f t="shared" si="2"/>
         <v>43965704</v>
       </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="I53">
+        <f t="shared" si="2"/>
+        <v>46585618</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="2"/>
+        <v>46615084</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="2"/>
+        <v>46575849</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="2"/>
+        <v>46611011</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="2"/>
+        <v>45663007</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="2"/>
+        <v>46570511</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="B54">
         <f>B53/$A$53</f>
         <v>0.75719017145182566</v>
@@ -1523,6 +1722,286 @@
       <c r="H54">
         <f>H53/$A$53</f>
         <v>0.72932320537235107</v>
+      </c>
+      <c r="I54">
+        <f>I53/$A$53</f>
+        <v>0.77278353700447733</v>
+      </c>
+      <c r="J54">
+        <f>J53/$A$53</f>
+        <v>0.77327233248855509</v>
+      </c>
+      <c r="K54">
+        <f>K53/$A$53</f>
+        <v>0.77262148436469058</v>
+      </c>
+      <c r="L54">
+        <f>L53/$A$53</f>
+        <v>0.7732047677017958</v>
+      </c>
+      <c r="M54">
+        <f>M53/$A$53</f>
+        <v>0.75747884378651376</v>
+      </c>
+      <c r="N54">
+        <f>N53/$A$53</f>
+        <v>0.77253293517939192</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="E59" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="F60">
+        <v>4</v>
+      </c>
+      <c r="G60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>20502785</v>
+      </c>
+      <c r="D61">
+        <v>68436</v>
+      </c>
+      <c r="E61">
+        <v>11683</v>
+      </c>
+      <c r="F61">
+        <v>157</v>
+      </c>
+      <c r="G61">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>385503</v>
+      </c>
+      <c r="D62">
+        <v>42782</v>
+      </c>
+      <c r="E62">
+        <v>11223</v>
+      </c>
+      <c r="F62">
+        <v>121</v>
+      </c>
+      <c r="G62">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63">
+        <v>3</v>
+      </c>
+      <c r="C63">
+        <v>476660</v>
+      </c>
+      <c r="D63">
+        <v>167613</v>
+      </c>
+      <c r="E63">
+        <v>195288</v>
+      </c>
+      <c r="F63">
+        <v>11007</v>
+      </c>
+      <c r="G63">
+        <v>2861</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64">
+        <v>11492</v>
+      </c>
+      <c r="D64">
+        <v>7467</v>
+      </c>
+      <c r="E64">
+        <v>50920</v>
+      </c>
+      <c r="F64">
+        <v>17726</v>
+      </c>
+      <c r="G64">
+        <v>5938</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>9221</v>
+      </c>
+      <c r="D65">
+        <v>3024</v>
+      </c>
+      <c r="E65">
+        <v>30824</v>
+      </c>
+      <c r="F65">
+        <v>31482</v>
+      </c>
+      <c r="G65">
+        <v>65890</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="E68" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <v>4</v>
+      </c>
+      <c r="G69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>20650981</v>
+      </c>
+      <c r="D70">
+        <v>81531</v>
+      </c>
+      <c r="E70">
+        <v>14611</v>
+      </c>
+      <c r="F70">
+        <v>190</v>
+      </c>
+      <c r="G70">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71">
+        <v>202</v>
+      </c>
+      <c r="D71">
+        <v>23</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>25</v>
+      </c>
+      <c r="B72">
+        <v>3</v>
+      </c>
+      <c r="C72">
+        <v>725433</v>
+      </c>
+      <c r="D72">
+        <v>204885</v>
+      </c>
+      <c r="E72">
+        <v>256164</v>
+      </c>
+      <c r="F72">
+        <v>29429</v>
+      </c>
+      <c r="G72">
+        <v>9046</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="C73">
+        <v>131</v>
+      </c>
+      <c r="D73">
+        <v>48</v>
+      </c>
+      <c r="E73">
+        <v>813</v>
+      </c>
+      <c r="F73">
+        <v>746</v>
+      </c>
+      <c r="G73">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="B74">
+        <v>5</v>
+      </c>
+      <c r="C74">
+        <v>8914</v>
+      </c>
+      <c r="D74">
+        <v>2835</v>
+      </c>
+      <c r="E74">
+        <v>28349</v>
+      </c>
+      <c r="F74">
+        <v>30128</v>
+      </c>
+      <c r="G74">
+        <v>65385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>